<commit_message>
Sanity Test -Profile Details
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPProject\Competitiontask1\MarsFramework\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPProject\Standard-task-Automation\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC42FF88-E8DD-4C53-B609-8B6608D47B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1B919-9833-457F-A568-E62FABA46AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -19,13 +19,15 @@
     <sheet name="SignIn" sheetId="1" r:id="rId4"/>
     <sheet name="ShareSkill" sheetId="4" r:id="rId5"/>
     <sheet name="Profile" sheetId="2" r:id="rId6"/>
+    <sheet name="ProfileDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="SearchSkill" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>Url</t>
   </si>
@@ -220,6 +222,33 @@
   </si>
   <si>
     <t>19:00:00 PM</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>Less than $500 per month</t>
+  </si>
+  <si>
+    <t>EarnTarget</t>
+  </si>
+  <si>
+    <t>Part Time</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -711,10 +740,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2C0763-148D-4F1B-AC04-51789190BC64}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -726,7 +755,7 @@
     <col min="8" max="9" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -775,8 +804,11 @@
       <c r="P1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -824,6 +856,9 @@
       </c>
       <c r="P2" t="s">
         <v>56</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -833,10 +868,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -846,7 +881,7 @@
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,8 +891,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -866,6 +904,9 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -883,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED40C2-E387-420A-8307-8C19194F1444}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
@@ -1088,4 +1129,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3CDB45-7BF6-4868-A0FA-04201470D259}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="22.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE46C633-0990-4FF4-8AD3-9847EED93ABB}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.36328125" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Neagative test cases for Certificate Included
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPProject\Standard-task-Automation\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586D0251-1F98-454B-971B-B99CAF43B055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8AC841-8FD7-47E4-AAB4-3F39B14BEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="880" yWindow="620" windowWidth="11170" windowHeight="9200" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>Url</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>NUS</t>
+  </si>
+  <si>
+    <t>NAFA</t>
+  </si>
+  <si>
+    <t>Painting</t>
   </si>
 </sst>
 </file>
@@ -757,10 +763,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30CE321-CCA4-4738-BDCE-458562EA6E38}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -805,6 +811,14 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>